<commit_message>
Some construction related files
</commit_message>
<xml_diff>
--- a/constructions/spacetypes and constrution colors.xlsx
+++ b/constructions/spacetypes and constrution colors.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="285" windowWidth="19320" windowHeight="12120"/>
+    <workbookView xWindow="360" yWindow="285" windowWidth="19320" windowHeight="12120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="spacetypes" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">spacetypes!$A$1:$O$113</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -455,8 +455,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1817,6 +1817,11 @@
       <color rgb="FF0D2BDD"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1895,6 +1900,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1929,6 +1935,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2104,15 +2111,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G118" sqref="G118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -2126,7 +2133,7 @@
     <col min="14" max="14" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -2155,7 +2162,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2198,7 +2205,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="3" spans="1:16" hidden="1">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2237,7 +2244,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:16" hidden="1">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2276,7 +2283,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:16" hidden="1">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2315,7 +2322,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:16" hidden="1">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2354,7 +2361,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:16" hidden="1">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -2393,7 +2400,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:16" hidden="1">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2432,7 +2439,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:16" hidden="1">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -2471,7 +2478,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:16" hidden="1">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2510,7 +2517,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:16" hidden="1">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2549,7 +2556,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2592,7 +2599,7 @@
         <v>0.68359375</v>
       </c>
     </row>
-    <row r="13" spans="1:16" hidden="1">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2631,7 +2638,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:16" hidden="1">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -2670,7 +2677,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:16" hidden="1">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -2709,7 +2716,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:16" hidden="1">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2748,7 +2755,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:16" hidden="1">
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2787,7 +2794,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:16" hidden="1">
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2826,7 +2833,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:16" hidden="1">
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2865,7 +2872,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2908,7 +2915,7 @@
         <v>0.5859375</v>
       </c>
     </row>
-    <row r="21" spans="1:16" hidden="1">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2947,7 +2954,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:16" hidden="1">
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2986,7 +2993,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:16" hidden="1">
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -3025,7 +3032,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -3067,7 +3074,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="25" spans="1:16" hidden="1">
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -3105,7 +3112,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1">
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -3143,7 +3150,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:16" hidden="1">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -3181,7 +3188,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1">
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -3219,7 +3226,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -3257,7 +3264,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -3299,7 +3306,7 @@
         <v>0.68359375</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -3338,7 +3345,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1">
+    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -3377,7 +3384,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1">
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -3416,7 +3423,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -3455,7 +3462,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -3494,7 +3501,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -3533,7 +3540,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -3576,7 +3583,7 @@
         <v>0.5859375</v>
       </c>
     </row>
-    <row r="38" spans="1:16" hidden="1">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -3615,7 +3622,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:16" hidden="1">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -3654,7 +3661,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:16" hidden="1">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -3693,7 +3700,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:16" hidden="1">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -3732,7 +3739,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:16" hidden="1">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -3771,7 +3778,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -3813,7 +3820,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="44" spans="1:16" hidden="1">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -3851,7 +3858,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:16" hidden="1">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -3889,7 +3896,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:16" hidden="1">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -3927,7 +3934,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:16" hidden="1">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -3965,7 +3972,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1">
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -4003,7 +4010,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1">
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -4041,7 +4048,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -4083,7 +4090,7 @@
         <v>0.68359375</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -4122,7 +4129,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:16" hidden="1">
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -4161,7 +4168,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1">
+    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -4200,7 +4207,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:16" hidden="1">
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -4239,7 +4246,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:16" hidden="1">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -4278,7 +4285,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:16" hidden="1">
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -4317,7 +4324,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:16" hidden="1">
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -4356,7 +4363,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:16" hidden="1">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -4395,7 +4402,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:16" hidden="1">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -4434,7 +4441,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:16" hidden="1">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -4473,7 +4480,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -4516,7 +4523,7 @@
         <v>0.5859375</v>
       </c>
     </row>
-    <row r="62" spans="1:16" hidden="1">
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -4555,7 +4562,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:16" hidden="1">
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -4594,7 +4601,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:16" hidden="1">
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>51</v>
       </c>
@@ -4633,7 +4640,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:16" hidden="1">
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -4672,7 +4679,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:16" hidden="1">
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -4711,7 +4718,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -4754,7 +4761,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="68" spans="1:16" hidden="1">
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>29</v>
       </c>
@@ -4793,7 +4800,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:16" hidden="1">
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -4832,7 +4839,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:16" hidden="1">
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>58</v>
       </c>
@@ -4871,7 +4878,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:16" hidden="1">
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -4910,7 +4917,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:16" hidden="1">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -4949,7 +4956,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:16" hidden="1">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -4988,7 +4995,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:16" hidden="1">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>57</v>
       </c>
@@ -5027,7 +5034,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -5069,7 +5076,7 @@
         <v>0.68359375</v>
       </c>
     </row>
-    <row r="76" spans="1:16" hidden="1">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>51</v>
       </c>
@@ -5107,7 +5114,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:16" hidden="1">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>58</v>
       </c>
@@ -5145,7 +5152,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:16" hidden="1">
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>29</v>
       </c>
@@ -5183,7 +5190,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:16" hidden="1">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -5221,7 +5228,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -5263,7 +5270,7 @@
         <v>0.5859375</v>
       </c>
     </row>
-    <row r="81" spans="1:16" hidden="1">
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -5302,7 +5309,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:16" hidden="1">
+    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -5341,7 +5348,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:16" hidden="1">
+    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -5380,7 +5387,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:16" hidden="1">
+    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>69</v>
       </c>
@@ -5419,7 +5426,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>29</v>
       </c>
@@ -5462,7 +5469,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="86" spans="1:16" hidden="1">
+    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>60</v>
       </c>
@@ -5501,7 +5508,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:16" hidden="1">
+    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>51</v>
       </c>
@@ -5540,7 +5547,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:16" hidden="1">
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>58</v>
       </c>
@@ -5579,7 +5586,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:16" hidden="1">
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>29</v>
       </c>
@@ -5618,7 +5625,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>58</v>
       </c>
@@ -5661,7 +5668,7 @@
         <v>0.68359375</v>
       </c>
     </row>
-    <row r="91" spans="1:16" hidden="1">
+    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -5700,7 +5707,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:16" hidden="1">
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>51</v>
       </c>
@@ -5739,7 +5746,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:16" hidden="1">
+    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>58</v>
       </c>
@@ -5778,7 +5785,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:16" hidden="1">
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>29</v>
       </c>
@@ -5817,7 +5824,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:16" hidden="1">
+    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>60</v>
       </c>
@@ -5856,7 +5863,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>29</v>
       </c>
@@ -5898,7 +5905,7 @@
         <v>0.5859375</v>
       </c>
     </row>
-    <row r="97" spans="1:16" hidden="1">
+    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>60</v>
       </c>
@@ -5936,7 +5943,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:16" hidden="1">
+    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>22</v>
       </c>
@@ -5974,7 +5981,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:16" hidden="1">
+    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>60</v>
       </c>
@@ -6012,7 +6019,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:16" hidden="1">
+    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -6050,7 +6057,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:16" hidden="1">
+    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>29</v>
       </c>
@@ -6088,7 +6095,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:16" hidden="1">
+    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -6126,7 +6133,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:16" hidden="1">
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>58</v>
       </c>
@@ -6164,7 +6171,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:16" hidden="1">
+    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>29</v>
       </c>
@@ -6202,7 +6209,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:16" hidden="1">
+    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>60</v>
       </c>
@@ -6240,7 +6247,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -6282,7 +6289,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="107" spans="1:16" hidden="1">
+    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -6321,7 +6328,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:16" hidden="1">
+    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>27</v>
       </c>
@@ -6360,7 +6367,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:16" hidden="1">
+    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>51</v>
       </c>
@@ -6399,7 +6406,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:16" hidden="1">
+    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>58</v>
       </c>
@@ -6438,7 +6445,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:16" hidden="1">
+    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>60</v>
       </c>
@@ -6477,7 +6484,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:16" hidden="1">
+    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>29</v>
       </c>
@@ -6516,7 +6523,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:15" hidden="1">
+    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>3</v>
       </c>
@@ -6555,7 +6562,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:15">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I114">
         <v>225</v>
       </c>
@@ -6569,7 +6576,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:15">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I116">
         <v>2009</v>
       </c>
@@ -6583,12 +6590,12 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I118" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I119">
         <v>200</v>
       </c>
@@ -6602,7 +6609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:15">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I120">
         <f>I119/256</f>
         <v>0.78125</v>
@@ -6622,9 +6629,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O113">
-    <filterColumn colId="9"/>
-    <filterColumn colId="10"/>
-    <filterColumn colId="11"/>
     <filterColumn colId="14">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -6640,21 +6644,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>109</v>
       </c>
@@ -6671,7 +6675,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
@@ -6696,7 +6700,7 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>124</v>
       </c>
@@ -6721,7 +6725,7 @@
         <v>0.5859375</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -6750,7 +6754,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -6775,7 +6779,7 @@
         <v>0.29296875</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -6800,7 +6804,7 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -6825,7 +6829,7 @@
         <v>0.5859375</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -6850,7 +6854,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -6875,7 +6879,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -6900,7 +6904,7 @@
         <v>0.87890625</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -6925,7 +6929,7 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -6950,7 +6954,7 @@
         <v>0.5859375</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>123</v>
       </c>
@@ -6975,7 +6979,7 @@
         <v>0.45703125</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -7000,7 +7004,7 @@
         <v>0.32421875</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>123</v>
       </c>
@@ -7025,7 +7029,7 @@
         <v>0.1953125</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>126</v>
       </c>
@@ -7050,7 +7054,7 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>126</v>
       </c>
@@ -7075,7 +7079,7 @@
         <v>0.5859375</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>126</v>
       </c>
@@ -7100,7 +7104,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>126</v>
       </c>
@@ -7125,7 +7129,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -7150,7 +7154,7 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -7175,7 +7179,7 @@
         <v>0.390625</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="84" t="s">
         <v>108</v>
       </c>
@@ -7183,7 +7187,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="85">
         <v>1</v>
       </c>
@@ -7197,7 +7201,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="85">
         <v>2</v>
       </c>
@@ -7209,7 +7213,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="85" t="s">
         <v>111</v>
       </c>
@@ -7221,7 +7225,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="85" t="s">
         <v>112</v>
       </c>
@@ -7233,7 +7237,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="85" t="s">
         <v>113</v>
       </c>
@@ -7245,7 +7249,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="85" t="s">
         <v>114</v>
       </c>
@@ -7257,7 +7261,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="85" t="s">
         <v>115</v>
       </c>
@@ -7269,7 +7273,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="85" t="s">
         <v>116</v>
       </c>
@@ -7281,7 +7285,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="85" t="s">
         <v>117</v>
       </c>
@@ -7293,7 +7297,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="85" t="s">
         <v>118</v>
       </c>
@@ -7305,7 +7309,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="85" t="s">
         <v>119</v>
       </c>
@@ -7317,7 +7321,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="85" t="s">
         <v>120</v>
       </c>
@@ -7329,7 +7333,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="85" t="s">
         <v>121</v>
       </c>
@@ -7341,7 +7345,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="85">
         <v>7</v>
       </c>
@@ -7353,7 +7357,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="85">
         <v>8</v>
       </c>
@@ -7364,30 +7368,30 @@
         <v>192</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="85"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="84" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="85">
         <v>1979</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="85">
         <v>1980</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="85">
         <v>2004</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="85">
         <v>2009</v>
       </c>

</xml_diff>